<commit_message>
add basic data references and flux box outline
</commit_message>
<xml_diff>
--- a/data_sources/defaults_Tables.xlsx
+++ b/data_sources/defaults_Tables.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nariv\OneDrive\JupyterN\streamlit_local\SoilsMassBalance\data_sources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>K</t>
   </si>
@@ -98,13 +103,16 @@
   </si>
   <si>
     <t>SP</t>
+  </si>
+  <si>
+    <t>Coarse_seds_subsurface</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +175,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -213,7 +229,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -245,9 +261,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,6 +296,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -454,19 +472,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,8 +527,11 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2.6</v>
       </c>
@@ -533,7 +554,7 @@
         <v>15500</v>
       </c>
       <c r="H2">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I2">
         <v>1133</v>
@@ -553,8 +574,11 @@
       <c r="N2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2.6</v>
       </c>
@@ -577,7 +601,7 @@
         <v>15500</v>
       </c>
       <c r="H3">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I3">
         <v>1133</v>
@@ -597,8 +621,11 @@
       <c r="N3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2.6</v>
       </c>
@@ -621,7 +648,7 @@
         <v>15500</v>
       </c>
       <c r="H4">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I4">
         <v>1133</v>
@@ -641,8 +668,11 @@
       <c r="N4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2.6</v>
       </c>
@@ -665,7 +695,7 @@
         <v>15500</v>
       </c>
       <c r="H5">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I5">
         <v>1133</v>
@@ -685,8 +715,11 @@
       <c r="N5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2.6</v>
       </c>
@@ -709,7 +742,7 @@
         <v>15500</v>
       </c>
       <c r="H6">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I6">
         <v>1133</v>
@@ -729,8 +762,11 @@
       <c r="N6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2.6</v>
       </c>
@@ -753,7 +789,7 @@
         <v>15500</v>
       </c>
       <c r="H7">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I7">
         <v>1133</v>
@@ -773,13 +809,16 @@
       <c r="N7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>14.6</v>
       </c>
       <c r="B8">
-        <v>962338.0959379557</v>
+        <v>962338.09593795566</v>
       </c>
       <c r="C8">
         <v>25</v>
@@ -797,7 +836,7 @@
         <v>15500</v>
       </c>
       <c r="H8">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I8">
         <v>1133</v>
@@ -817,13 +856,16 @@
       <c r="N8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>14.6</v>
       </c>
       <c r="B9">
-        <v>962338.0959379557</v>
+        <v>962338.09593795566</v>
       </c>
       <c r="C9">
         <v>25</v>
@@ -841,7 +883,7 @@
         <v>15500</v>
       </c>
       <c r="H9">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I9">
         <v>1133</v>
@@ -861,13 +903,16 @@
       <c r="N9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>14.6</v>
       </c>
       <c r="B10">
-        <v>962338.0959379557</v>
+        <v>962338.09593795566</v>
       </c>
       <c r="C10">
         <v>25</v>
@@ -885,7 +930,7 @@
         <v>15500</v>
       </c>
       <c r="H10">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I10">
         <v>1133</v>
@@ -905,13 +950,16 @@
       <c r="N10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>14.6</v>
       </c>
       <c r="B11">
-        <v>962338.0959379557</v>
+        <v>962338.09593795566</v>
       </c>
       <c r="C11">
         <v>25</v>
@@ -929,7 +977,7 @@
         <v>15500</v>
       </c>
       <c r="H11">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I11">
         <v>1133</v>
@@ -949,13 +997,16 @@
       <c r="N11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>14.6</v>
       </c>
       <c r="B12">
-        <v>962338.0959379557</v>
+        <v>962338.09593795566</v>
       </c>
       <c r="C12">
         <v>25</v>
@@ -973,7 +1024,7 @@
         <v>15500</v>
       </c>
       <c r="H12">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I12">
         <v>1133</v>
@@ -992,6 +1043,9 @@
       </c>
       <c r="N12" t="s">
         <v>27</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>